<commit_message>
Fixed data entry error
</commit_message>
<xml_diff>
--- a/Data/2018 Lake Mattamuskeet Data from ISB Lab.xlsx
+++ b/Data/2018 Lake Mattamuskeet Data from ISB Lab.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\USERS\DAOWEN\DESKTOP\2018 MATTAMUSKEET\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmoorman\Documents\I&amp;m\Refuge Visits\Mattamuskeet\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18585" windowHeight="11820"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10500"/>
   </bookViews>
   <sheets>
     <sheet name="FlatData" sheetId="1" r:id="rId1"/>
@@ -1107,7 +1107,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U209"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A177" workbookViewId="0">
+      <selection activeCell="D119" sqref="C119:D131"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -8810,10 +8812,10 @@
         <v>122</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>23</v>
+        <v>94</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>24</v>
+        <v>95</v>
       </c>
       <c r="E119" s="2">
         <v>43252</v>
@@ -8875,10 +8877,10 @@
         <v>122</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>23</v>
+        <v>94</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>24</v>
+        <v>95</v>
       </c>
       <c r="E120" s="2">
         <v>43252</v>
@@ -8940,10 +8942,10 @@
         <v>122</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>23</v>
+        <v>94</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>24</v>
+        <v>95</v>
       </c>
       <c r="E121" s="2">
         <v>43252</v>
@@ -9005,10 +9007,10 @@
         <v>122</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>23</v>
+        <v>94</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>24</v>
+        <v>95</v>
       </c>
       <c r="E122" s="2">
         <v>43252</v>
@@ -9070,10 +9072,10 @@
         <v>122</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>23</v>
+        <v>94</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>24</v>
+        <v>95</v>
       </c>
       <c r="E123" s="2">
         <v>43252</v>
@@ -9135,10 +9137,10 @@
         <v>122</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>23</v>
+        <v>94</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>24</v>
+        <v>95</v>
       </c>
       <c r="E124" s="2">
         <v>43252</v>
@@ -9200,10 +9202,10 @@
         <v>122</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>23</v>
+        <v>94</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>24</v>
+        <v>95</v>
       </c>
       <c r="E125" s="2">
         <v>43252</v>
@@ -9265,10 +9267,10 @@
         <v>122</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>23</v>
+        <v>94</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>24</v>
+        <v>95</v>
       </c>
       <c r="E126" s="2">
         <v>43252</v>
@@ -9330,10 +9332,10 @@
         <v>122</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>23</v>
+        <v>94</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>24</v>
+        <v>95</v>
       </c>
       <c r="E127" s="2">
         <v>43252</v>
@@ -9395,10 +9397,10 @@
         <v>122</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>23</v>
+        <v>94</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>24</v>
+        <v>95</v>
       </c>
       <c r="E128" s="2">
         <v>43252</v>
@@ -9460,10 +9462,10 @@
         <v>122</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>23</v>
+        <v>94</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>24</v>
+        <v>95</v>
       </c>
       <c r="E129" s="2">
         <v>43252</v>
@@ -9525,10 +9527,10 @@
         <v>122</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>23</v>
+        <v>94</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>24</v>
+        <v>95</v>
       </c>
       <c r="E130" s="2">
         <v>43252</v>
@@ -9590,10 +9592,10 @@
         <v>122</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>23</v>
+        <v>94</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>24</v>
+        <v>95</v>
       </c>
       <c r="E131" s="2">
         <v>43252</v>

</xml_diff>